<commit_message>
adding school shooting, static files
</commit_message>
<xml_diff>
--- a/2018/febsnow/snow.xlsx
+++ b/2018/febsnow/snow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8000" windowHeight="15100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19840" windowHeight="15100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -714,9 +714,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J16" sqref="J16"/>
+      <selection pane="topRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -749,7 +749,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="H2">
-        <v>7.3</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -764,7 +764,7 @@
         <v>4.8</v>
       </c>
       <c r="H3">
-        <v>6.8</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1022,7 +1022,7 @@
         <v>-88.09</v>
       </c>
       <c r="H21">
-        <v>8.5</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="22" spans="1:8">

</xml_diff>